<commit_message>
before messing with formatting
</commit_message>
<xml_diff>
--- a/Reports/Lobewise Comparisons/ResultsFinal/ggo.xlsx
+++ b/Reports/Lobewise Comparisons/ResultsFinal/ggo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3c2d16a148962151/Desktop/BIOSTAT/Thesis/Thesis/Reports/Lobewise Comparisons/ResultsFinal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="11_F25DC773A252ABDACC1048CA799F592E5BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E583E0FB-E302-4DE9-A5BB-606FF38F2787}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="11_F25DC773A252ABDACC1048CA799F592E5BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77016349-EA53-4117-8353-C7DFB5416287}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PO_main" sheetId="1" r:id="rId1"/>
@@ -837,7 +837,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -900,12 +900,12 @@
         <v>3.0270008475602372</v>
       </c>
       <c r="C3">
+        <f>1/0.60858</f>
+        <v>1.643169345032699</v>
+      </c>
+      <c r="D3">
         <f>1/0.17933</f>
         <v>5.5763118273573857</v>
-      </c>
-      <c r="D3">
-        <f>1/0.60858</f>
-        <v>1.643169345032699</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1018,12 +1018,12 @@
         <v>1.7958479994253287</v>
       </c>
       <c r="C8">
+        <f>1/1.0531</f>
+        <v>0.94957743804007222</v>
+      </c>
+      <c r="D8">
         <f>1/0.29443</f>
         <v>3.3963930306015011</v>
-      </c>
-      <c r="D8">
-        <f>1/1.0531</f>
-        <v>0.94957743804007222</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1044,12 +1044,12 @@
         <v>1.7507615812878601</v>
       </c>
       <c r="C9">
+        <f>1/1.07933</f>
+        <v>0.92650069950802827</v>
+      </c>
+      <c r="D9">
         <f>1/0.30227</f>
         <v>3.3083005260197837</v>
-      </c>
-      <c r="D9">
-        <f>1/1.07933</f>
-        <v>0.92650069950802827</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1070,12 +1070,12 @@
         <v>1.4742087184703612</v>
       </c>
       <c r="C10">
+        <f>1/1.174</f>
+        <v>0.85178875638841567</v>
+      </c>
+      <c r="D10">
         <f>1/0.39194</f>
         <v>2.5514109302444252</v>
-      </c>
-      <c r="D10">
-        <f>1/1.174</f>
-        <v>0.85178875638841567</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1096,12 +1096,12 @@
         <v>1.4576197070184387</v>
       </c>
       <c r="C11">
+        <f>1/1.32001</f>
+        <v>0.75757001840895155</v>
+      </c>
+      <c r="D11">
         <f>1/0.35656</f>
         <v>2.8045770697778778</v>
-      </c>
-      <c r="D11">
-        <f>1/1.32001</f>
-        <v>0.75757001840895155</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1168,12 +1168,12 @@
         <v>1.2320429736589211</v>
       </c>
       <c r="C14">
+        <f>1/1.49179</f>
+        <v>0.67033563705347265</v>
+      </c>
+      <c r="D14">
         <f>1/0.44161</f>
         <v>2.2644414755100652</v>
-      </c>
-      <c r="D14">
-        <f>1/1.49179</f>
-        <v>0.67033563705347265</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1217,12 +1217,12 @@
         <v>1.0257567520438202</v>
       </c>
       <c r="C16">
+        <f>1/1.91611</f>
+        <v>0.5218907056484231</v>
+      </c>
+      <c r="D16">
         <f>1/0.49601</f>
         <v>2.0160883853148124</v>
-      </c>
-      <c r="D16">
-        <f>1/1.91611</f>
-        <v>0.5218907056484231</v>
       </c>
       <c r="E16">
         <v>0</v>

</xml_diff>